<commit_message>
Remplissage des différents onglets.
Suppression des onglets non utilisés.
</commit_message>
<xml_diff>
--- a/files/templateEdit.xlsx
+++ b/files/templateEdit.xlsx
@@ -5,14 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sum_Chromosome" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sum_Mitochondrion" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Sum_Chloroplast" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Sum_Chloroplast" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sum_Chromosome" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Complete_Genome" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Sum_DNA" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Sum_Linkage" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Sum_Mitochondrion" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="106">
   <si>
     <t xml:space="preserve">Information</t>
   </si>
@@ -339,6 +341,9 @@
   </si>
   <si>
     <t xml:space="preserve">TCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statistiques dinucléotides</t>
   </si>
 </sst>
 </file>
@@ -678,9 +683,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -819,16 +824,16 @@
   </sheetPr>
   <dimension ref="A1:T66"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="12" min="2" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="2" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -884,7 +889,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>21</v>
       </c>
@@ -946,7 +951,7 @@
       <c r="S5" s="19"/>
       <c r="T5" s="19"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
         <v>29</v>
       </c>
@@ -1008,7 +1013,7 @@
       <c r="S9" s="19"/>
       <c r="T9" s="19"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
         <v>37</v>
       </c>
@@ -1070,7 +1075,7 @@
       <c r="S13" s="19"/>
       <c r="T13" s="19"/>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
         <v>45</v>
       </c>
@@ -1132,7 +1137,7 @@
       <c r="S17" s="19"/>
       <c r="T17" s="19"/>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
         <v>53</v>
       </c>
@@ -1156,7 +1161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="18" t="s">
         <v>55</v>
       </c>
@@ -1170,12 +1175,12 @@
       <c r="J19" s="19"/>
       <c r="K19" s="19"/>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="18" t="s">
         <v>57</v>
       </c>
@@ -1189,12 +1194,12 @@
       <c r="J21" s="19"/>
       <c r="K21" s="19"/>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="18" t="s">
         <v>59</v>
       </c>
@@ -1211,19 +1216,19 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
         <v>61</v>
       </c>
       <c r="M24" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="N24" s="18" t="str">
+      <c r="N24" s="18" t="n">
         <f aca="false">'General Information'!B7</f>
         <v>123123123</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="18" t="s">
         <v>63</v>
       </c>
@@ -1239,17 +1244,17 @@
       <c r="M25" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="N25" s="18" t="str">
+      <c r="N25" s="18" t="n">
         <f aca="false">'General Information'!B9</f>
         <v>1234</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="18" t="s">
         <v>66</v>
       </c>
@@ -1263,12 +1268,12 @@
       <c r="J27" s="19"/>
       <c r="K27" s="19"/>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="18" t="s">
         <v>68</v>
       </c>
@@ -1282,12 +1287,12 @@
       <c r="J29" s="19"/>
       <c r="K29" s="19"/>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="18" t="s">
         <v>70</v>
       </c>
@@ -1301,12 +1306,12 @@
       <c r="J31" s="19"/>
       <c r="K31" s="19"/>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="18" t="s">
         <v>72</v>
       </c>
@@ -1320,12 +1325,12 @@
       <c r="J33" s="19"/>
       <c r="K33" s="19"/>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="18" t="s">
         <v>74</v>
       </c>
@@ -1339,12 +1344,12 @@
       <c r="J35" s="19"/>
       <c r="K35" s="19"/>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="18" t="s">
         <v>76</v>
       </c>
@@ -1358,12 +1363,12 @@
       <c r="J37" s="19"/>
       <c r="K37" s="19"/>
     </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="18" t="s">
         <v>78</v>
       </c>
@@ -1377,12 +1382,12 @@
       <c r="J39" s="19"/>
       <c r="K39" s="19"/>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="18" t="s">
         <v>80</v>
       </c>
@@ -1396,12 +1401,12 @@
       <c r="J41" s="19"/>
       <c r="K41" s="19"/>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="18" t="s">
         <v>82</v>
       </c>
@@ -1415,12 +1420,12 @@
       <c r="J43" s="19"/>
       <c r="K43" s="19"/>
     </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="18" t="s">
         <v>84</v>
       </c>
@@ -1434,12 +1439,12 @@
       <c r="J45" s="19"/>
       <c r="K45" s="19"/>
     </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="18" t="s">
         <v>86</v>
       </c>
@@ -1453,12 +1458,12 @@
       <c r="J47" s="19"/>
       <c r="K47" s="19"/>
     </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="18" t="s">
         <v>88</v>
       </c>
@@ -1472,12 +1477,12 @@
       <c r="J49" s="19"/>
       <c r="K49" s="19"/>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="18" t="s">
         <v>90</v>
       </c>
@@ -1491,12 +1496,12 @@
       <c r="J51" s="19"/>
       <c r="K51" s="19"/>
     </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="18" t="s">
         <v>92</v>
       </c>
@@ -1510,12 +1515,12 @@
       <c r="J53" s="19"/>
       <c r="K53" s="19"/>
     </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="18" t="s">
         <v>94</v>
       </c>
@@ -1529,12 +1534,12 @@
       <c r="J55" s="19"/>
       <c r="K55" s="19"/>
     </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="18" t="s">
         <v>96</v>
       </c>
@@ -1548,12 +1553,12 @@
       <c r="J57" s="19"/>
       <c r="K57" s="19"/>
     </row>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="18" t="s">
         <v>98</v>
       </c>
@@ -1567,12 +1572,12 @@
       <c r="J59" s="19"/>
       <c r="K59" s="19"/>
     </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="18" t="s">
         <v>100</v>
       </c>
@@ -1586,12 +1591,12 @@
       <c r="J61" s="19"/>
       <c r="K61" s="19"/>
     </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="18" t="s">
         <v>102</v>
       </c>
@@ -1605,12 +1610,12 @@
       <c r="J63" s="19"/>
       <c r="K63" s="19"/>
     </row>
-    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="18" t="s">
         <v>104</v>
       </c>
@@ -1672,15 +1677,15 @@
   <dimension ref="A1:T66"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="12" min="2" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="2" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1736,7 +1741,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>21</v>
       </c>
@@ -1798,7 +1803,7 @@
       <c r="S5" s="19"/>
       <c r="T5" s="19"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
         <v>29</v>
       </c>
@@ -1860,7 +1865,7 @@
       <c r="S9" s="19"/>
       <c r="T9" s="19"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
         <v>37</v>
       </c>
@@ -1922,7 +1927,7 @@
       <c r="S13" s="19"/>
       <c r="T13" s="19"/>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
         <v>45</v>
       </c>
@@ -1984,7 +1989,7 @@
       <c r="S17" s="19"/>
       <c r="T17" s="19"/>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
         <v>53</v>
       </c>
@@ -2008,7 +2013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="18" t="s">
         <v>55</v>
       </c>
@@ -2022,12 +2027,12 @@
       <c r="J19" s="19"/>
       <c r="K19" s="19"/>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="18" t="s">
         <v>57</v>
       </c>
@@ -2041,12 +2046,12 @@
       <c r="J21" s="19"/>
       <c r="K21" s="19"/>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="18" t="s">
         <v>59</v>
       </c>
@@ -2063,19 +2068,19 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
         <v>61</v>
       </c>
       <c r="M24" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="N24" s="18" t="str">
+      <c r="N24" s="18" t="n">
         <f aca="false">'General Information'!B7</f>
         <v>123123123</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="18" t="s">
         <v>63</v>
       </c>
@@ -2091,17 +2096,17 @@
       <c r="M25" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="N25" s="18" t="str">
+      <c r="N25" s="18" t="n">
         <f aca="false">'General Information'!B9</f>
         <v>1234</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="18" t="s">
         <v>66</v>
       </c>
@@ -2115,12 +2120,12 @@
       <c r="J27" s="19"/>
       <c r="K27" s="19"/>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="18" t="s">
         <v>68</v>
       </c>
@@ -2134,12 +2139,12 @@
       <c r="J29" s="19"/>
       <c r="K29" s="19"/>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="18" t="s">
         <v>70</v>
       </c>
@@ -2153,12 +2158,12 @@
       <c r="J31" s="19"/>
       <c r="K31" s="19"/>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="18" t="s">
         <v>72</v>
       </c>
@@ -2172,12 +2177,12 @@
       <c r="J33" s="19"/>
       <c r="K33" s="19"/>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="18" t="s">
         <v>74</v>
       </c>
@@ -2191,12 +2196,12 @@
       <c r="J35" s="19"/>
       <c r="K35" s="19"/>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="18" t="s">
         <v>76</v>
       </c>
@@ -2210,12 +2215,12 @@
       <c r="J37" s="19"/>
       <c r="K37" s="19"/>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="18" t="s">
         <v>78</v>
       </c>
@@ -2229,12 +2234,12 @@
       <c r="J39" s="19"/>
       <c r="K39" s="19"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="18" t="s">
         <v>80</v>
       </c>
@@ -2248,12 +2253,12 @@
       <c r="J41" s="19"/>
       <c r="K41" s="19"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="18" t="s">
         <v>82</v>
       </c>
@@ -2267,12 +2272,12 @@
       <c r="J43" s="19"/>
       <c r="K43" s="19"/>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="18" t="s">
         <v>84</v>
       </c>
@@ -2286,12 +2291,12 @@
       <c r="J45" s="19"/>
       <c r="K45" s="19"/>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="18" t="s">
         <v>86</v>
       </c>
@@ -2305,12 +2310,12 @@
       <c r="J47" s="19"/>
       <c r="K47" s="19"/>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="18" t="s">
         <v>88</v>
       </c>
@@ -2324,12 +2329,12 @@
       <c r="J49" s="19"/>
       <c r="K49" s="19"/>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="18" t="s">
         <v>90</v>
       </c>
@@ -2343,12 +2348,12 @@
       <c r="J51" s="19"/>
       <c r="K51" s="19"/>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="18" t="s">
         <v>92</v>
       </c>
@@ -2362,12 +2367,12 @@
       <c r="J53" s="19"/>
       <c r="K53" s="19"/>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="18" t="s">
         <v>94</v>
       </c>
@@ -2381,12 +2386,12 @@
       <c r="J55" s="19"/>
       <c r="K55" s="19"/>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="18" t="s">
         <v>96</v>
       </c>
@@ -2400,12 +2405,12 @@
       <c r="J57" s="19"/>
       <c r="K57" s="19"/>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="18" t="s">
         <v>98</v>
       </c>
@@ -2419,12 +2424,12 @@
       <c r="J59" s="19"/>
       <c r="K59" s="19"/>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="18" t="s">
         <v>100</v>
       </c>
@@ -2438,12 +2443,12 @@
       <c r="J61" s="19"/>
       <c r="K61" s="19"/>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="18" t="s">
         <v>102</v>
       </c>
@@ -2457,12 +2462,12 @@
       <c r="J63" s="19"/>
       <c r="K63" s="19"/>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="18" t="s">
         <v>104</v>
       </c>
@@ -2524,15 +2529,15 @@
   <dimension ref="A1:T66"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="12" min="2" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="2" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2588,7 +2593,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>21</v>
       </c>
@@ -2650,7 +2655,7 @@
       <c r="S5" s="19"/>
       <c r="T5" s="19"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
         <v>29</v>
       </c>
@@ -2712,7 +2717,7 @@
       <c r="S9" s="19"/>
       <c r="T9" s="19"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
         <v>37</v>
       </c>
@@ -2774,7 +2779,7 @@
       <c r="S13" s="19"/>
       <c r="T13" s="19"/>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
         <v>45</v>
       </c>
@@ -2836,7 +2841,7 @@
       <c r="S17" s="19"/>
       <c r="T17" s="19"/>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
         <v>53</v>
       </c>
@@ -2860,7 +2865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="18" t="s">
         <v>55</v>
       </c>
@@ -2874,12 +2879,12 @@
       <c r="J19" s="19"/>
       <c r="K19" s="19"/>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="18" t="s">
         <v>57</v>
       </c>
@@ -2893,12 +2898,12 @@
       <c r="J21" s="19"/>
       <c r="K21" s="19"/>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="18" t="s">
         <v>59</v>
       </c>
@@ -2915,19 +2920,19 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
         <v>61</v>
       </c>
       <c r="M24" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="N24" s="18" t="str">
+      <c r="N24" s="18" t="n">
         <f aca="false">'General Information'!B7</f>
         <v>123123123</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="18" t="s">
         <v>63</v>
       </c>
@@ -2943,17 +2948,17 @@
       <c r="M25" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="N25" s="18" t="str">
+      <c r="N25" s="18" t="n">
         <f aca="false">'General Information'!B9</f>
         <v>1234</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="18" t="s">
         <v>66</v>
       </c>
@@ -2967,12 +2972,12 @@
       <c r="J27" s="19"/>
       <c r="K27" s="19"/>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="18" t="s">
         <v>68</v>
       </c>
@@ -2986,12 +2991,12 @@
       <c r="J29" s="19"/>
       <c r="K29" s="19"/>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="18" t="s">
         <v>70</v>
       </c>
@@ -3005,12 +3010,12 @@
       <c r="J31" s="19"/>
       <c r="K31" s="19"/>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="18" t="s">
         <v>72</v>
       </c>
@@ -3024,12 +3029,12 @@
       <c r="J33" s="19"/>
       <c r="K33" s="19"/>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="18" t="s">
         <v>74</v>
       </c>
@@ -3043,12 +3048,12 @@
       <c r="J35" s="19"/>
       <c r="K35" s="19"/>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="18" t="s">
         <v>76</v>
       </c>
@@ -3062,12 +3067,12 @@
       <c r="J37" s="19"/>
       <c r="K37" s="19"/>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="18" t="s">
         <v>78</v>
       </c>
@@ -3081,12 +3086,12 @@
       <c r="J39" s="19"/>
       <c r="K39" s="19"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="18" t="s">
         <v>80</v>
       </c>
@@ -3100,12 +3105,12 @@
       <c r="J41" s="19"/>
       <c r="K41" s="19"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="18" t="s">
         <v>82</v>
       </c>
@@ -3119,12 +3124,12 @@
       <c r="J43" s="19"/>
       <c r="K43" s="19"/>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="18" t="s">
         <v>84</v>
       </c>
@@ -3138,12 +3143,12 @@
       <c r="J45" s="19"/>
       <c r="K45" s="19"/>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="18" t="s">
         <v>86</v>
       </c>
@@ -3157,12 +3162,12 @@
       <c r="J47" s="19"/>
       <c r="K47" s="19"/>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="18" t="s">
         <v>88</v>
       </c>
@@ -3176,12 +3181,12 @@
       <c r="J49" s="19"/>
       <c r="K49" s="19"/>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="18" t="s">
         <v>90</v>
       </c>
@@ -3195,12 +3200,12 @@
       <c r="J51" s="19"/>
       <c r="K51" s="19"/>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="18" t="s">
         <v>92</v>
       </c>
@@ -3214,12 +3219,12 @@
       <c r="J53" s="19"/>
       <c r="K53" s="19"/>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="18" t="s">
         <v>94</v>
       </c>
@@ -3233,12 +3238,12 @@
       <c r="J55" s="19"/>
       <c r="K55" s="19"/>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="18" t="s">
         <v>96</v>
       </c>
@@ -3252,12 +3257,12 @@
       <c r="J57" s="19"/>
       <c r="K57" s="19"/>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="18" t="s">
         <v>98</v>
       </c>
@@ -3271,12 +3276,12 @@
       <c r="J59" s="19"/>
       <c r="K59" s="19"/>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="18" t="s">
         <v>100</v>
       </c>
@@ -3290,12 +3295,12 @@
       <c r="J61" s="19"/>
       <c r="K61" s="19"/>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="18" t="s">
         <v>102</v>
       </c>
@@ -3309,12 +3314,12 @@
       <c r="J63" s="19"/>
       <c r="K63" s="19"/>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="18" t="s">
         <v>104</v>
       </c>
@@ -3381,10 +3386,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="12" min="2" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="2" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3774,7 +3779,7 @@
       <c r="M24" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="N24" s="18" t="str">
+      <c r="N24" s="18" t="n">
         <f aca="false">'General Information'!B7</f>
         <v>123123123</v>
       </c>
@@ -3795,7 +3800,1711 @@
       <c r="M25" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="N25" s="18" t="str">
+      <c r="N25" s="18" t="n">
+        <f aca="false">'General Information'!B9</f>
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="19"/>
+      <c r="K47" s="19"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="19"/>
+      <c r="I49" s="19"/>
+      <c r="J49" s="19"/>
+      <c r="K49" s="19"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="19"/>
+      <c r="K51" s="19"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="19"/>
+      <c r="J53" s="19"/>
+      <c r="K53" s="19"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="19"/>
+      <c r="K55" s="19"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="19"/>
+      <c r="K57" s="19"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" s="19"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="19"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="19"/>
+      <c r="J59" s="19"/>
+      <c r="K59" s="19"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61" s="19"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="19"/>
+      <c r="I61" s="19"/>
+      <c r="J61" s="19"/>
+      <c r="K61" s="19"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
+      <c r="J63" s="19"/>
+      <c r="K63" s="19"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C65" s="19"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="19"/>
+      <c r="F65" s="19"/>
+      <c r="G65" s="19"/>
+      <c r="H65" s="19"/>
+      <c r="I65" s="19"/>
+      <c r="J65" s="19"/>
+      <c r="K65" s="19"/>
+    </row>
+    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C66" s="21" t="n">
+        <f aca="false">SUM(C2:C65)</f>
+        <v>0</v>
+      </c>
+      <c r="D66" s="21" t="n">
+        <f aca="false">SUM(D2:D65)</f>
+        <v>0</v>
+      </c>
+      <c r="E66" s="21" t="n">
+        <f aca="false">SUM(E2:E65)</f>
+        <v>0</v>
+      </c>
+      <c r="F66" s="21" t="n">
+        <f aca="false">SUM(F2:F65)</f>
+        <v>0</v>
+      </c>
+      <c r="G66" s="21" t="n">
+        <f aca="false">SUM(G2:G65)</f>
+        <v>0</v>
+      </c>
+      <c r="H66" s="21" t="n">
+        <f aca="false">SUM(H2:H65)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:T66"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8673469387755"/>
+    <col collapsed="false" hidden="false" max="12" min="2" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="24.4489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="13.6326530612245"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="N3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="N5" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="N7" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="N9" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="N11" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="N12" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="N13" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="N14" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="N15" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="N16" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="N17" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="N18" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="O18" s="21" t="n">
+        <f aca="false">SUM(O2:O17)</f>
+        <v>0</v>
+      </c>
+      <c r="P18" s="21" t="n">
+        <f aca="false">SUM(P2:P17)</f>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="21" t="n">
+        <f aca="false">SUM(Q2:Q17)</f>
+        <v>0</v>
+      </c>
+      <c r="R18" s="21" t="n">
+        <f aca="false">SUM(R2:R17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="M23" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="M24" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="N24" s="18" t="n">
+        <f aca="false">'General Information'!B7</f>
+        <v>123123123</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="M25" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="N25" s="18" t="n">
+        <f aca="false">'General Information'!B9</f>
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="19"/>
+      <c r="K47" s="19"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="19"/>
+      <c r="I49" s="19"/>
+      <c r="J49" s="19"/>
+      <c r="K49" s="19"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="19"/>
+      <c r="K51" s="19"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="19"/>
+      <c r="J53" s="19"/>
+      <c r="K53" s="19"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="19"/>
+      <c r="K55" s="19"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="19"/>
+      <c r="K57" s="19"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" s="19"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="19"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="19"/>
+      <c r="J59" s="19"/>
+      <c r="K59" s="19"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61" s="19"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="19"/>
+      <c r="I61" s="19"/>
+      <c r="J61" s="19"/>
+      <c r="K61" s="19"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
+      <c r="J63" s="19"/>
+      <c r="K63" s="19"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C65" s="19"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="19"/>
+      <c r="F65" s="19"/>
+      <c r="G65" s="19"/>
+      <c r="H65" s="19"/>
+      <c r="I65" s="19"/>
+      <c r="J65" s="19"/>
+      <c r="K65" s="19"/>
+    </row>
+    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C66" s="21" t="n">
+        <f aca="false">SUM(C2:C65)</f>
+        <v>0</v>
+      </c>
+      <c r="D66" s="21" t="n">
+        <f aca="false">SUM(D2:D65)</f>
+        <v>0</v>
+      </c>
+      <c r="E66" s="21" t="n">
+        <f aca="false">SUM(E2:E65)</f>
+        <v>0</v>
+      </c>
+      <c r="F66" s="21" t="n">
+        <f aca="false">SUM(F2:F65)</f>
+        <v>0</v>
+      </c>
+      <c r="G66" s="21" t="n">
+        <f aca="false">SUM(G2:G65)</f>
+        <v>0</v>
+      </c>
+      <c r="H66" s="21" t="n">
+        <f aca="false">SUM(H2:H65)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:T66"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="2" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="13.6326530612245"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="N3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="N5" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="N7" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="N9" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="N11" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="N12" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="N13" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="N14" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="N15" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="N16" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="N17" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="N18" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="O18" s="21" t="n">
+        <f aca="false">SUM(O2:O17)</f>
+        <v>0</v>
+      </c>
+      <c r="P18" s="21" t="n">
+        <f aca="false">SUM(P2:P17)</f>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="21" t="n">
+        <f aca="false">SUM(Q2:Q17)</f>
+        <v>0</v>
+      </c>
+      <c r="R18" s="21" t="n">
+        <f aca="false">SUM(R2:R17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="M23" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="M24" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="N24" s="18" t="n">
+        <f aca="false">'General Information'!B7</f>
+        <v>123123123</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="M25" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="N25" s="18" t="n">
         <f aca="false">'General Information'!B9</f>
         <v>1234</v>
       </c>

</xml_diff>

<commit_message>
Corrections mineurs sur l'écriture des excel
Meilleure mise en page du template
</commit_message>
<xml_diff>
--- a/files/templateEdit.xlsx
+++ b/files/templateEdit.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="106">
   <si>
     <t xml:space="preserve">Information</t>
   </si>
@@ -86,6 +86,9 @@
     <t xml:space="preserve">Pref Phase 2</t>
   </si>
   <si>
+    <t xml:space="preserve">Statistiques dinucléotides</t>
+  </si>
+  <si>
     <t xml:space="preserve">AAA</t>
   </si>
   <si>
@@ -215,7 +218,7 @@
     <t xml:space="preserve">TAC</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of invalid csd</t>
+    <t xml:space="preserve">Number of invalid cds</t>
   </si>
   <si>
     <t xml:space="preserve">AAG</t>
@@ -669,17 +672,18 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8673469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -818,21 +822,31 @@
   </sheetPr>
   <dimension ref="A1:T66"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M24" activeCellId="0" sqref="M24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.87755102040816"/>
-    <col collapsed="false" hidden="false" max="12" min="3" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="24.8673469387755"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.780612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0561224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6377551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.1938775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.780612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="12.9132653061225"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.5"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.780612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.780612244898"/>
+    <col collapsed="false" hidden="false" max="20" min="16" style="0" width="12.9132653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
@@ -864,7 +878,7 @@
         <v>20</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="O1" s="16" t="s">
         <v>12</v>
@@ -887,15 +901,15 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
@@ -907,7 +921,7 @@
       <c r="J3" s="19"/>
       <c r="K3" s="19"/>
       <c r="N3" s="16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O3" s="19"/>
       <c r="P3" s="19"/>
@@ -918,15 +932,15 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
@@ -938,7 +952,7 @@
       <c r="J5" s="19"/>
       <c r="K5" s="19"/>
       <c r="N5" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O5" s="19"/>
       <c r="P5" s="19"/>
@@ -949,15 +963,15 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N6" s="17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
@@ -969,7 +983,7 @@
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
       <c r="N7" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O7" s="19"/>
       <c r="P7" s="19"/>
@@ -980,15 +994,15 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N8" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
@@ -1000,7 +1014,7 @@
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
       <c r="N9" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O9" s="19"/>
       <c r="P9" s="19"/>
@@ -1011,15 +1025,15 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
@@ -1031,7 +1045,7 @@
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
       <c r="N11" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O11" s="19"/>
       <c r="P11" s="19"/>
@@ -1042,15 +1056,15 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N12" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
@@ -1062,7 +1076,7 @@
       <c r="J13" s="19"/>
       <c r="K13" s="19"/>
       <c r="N13" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="O13" s="19"/>
       <c r="P13" s="19"/>
@@ -1073,15 +1087,15 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N14" s="17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
@@ -1093,7 +1107,7 @@
       <c r="J15" s="19"/>
       <c r="K15" s="19"/>
       <c r="N15" s="16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="O15" s="19"/>
       <c r="P15" s="19"/>
@@ -1104,15 +1118,15 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N16" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
@@ -1124,7 +1138,7 @@
       <c r="J17" s="19"/>
       <c r="K17" s="19"/>
       <c r="N17" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="O17" s="19"/>
       <c r="P17" s="19"/>
@@ -1135,10 +1149,10 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N18" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="O18" s="21" t="n">
         <f aca="false">SUM(O2:O17)</f>
@@ -1159,7 +1173,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
@@ -1173,12 +1187,12 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
@@ -1192,12 +1206,12 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C23" s="19"/>
       <c r="D23" s="19"/>
@@ -1209,24 +1223,23 @@
       <c r="J23" s="19"/>
       <c r="K23" s="19"/>
       <c r="M23" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M24" s="22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N24" s="18" t="n">
-        <f aca="false">'General Information'!B7</f>
-        <v>123123123</v>
+        <v>42424242</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
@@ -1238,21 +1251,20 @@
       <c r="J25" s="19"/>
       <c r="K25" s="19"/>
       <c r="M25" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N25" s="18" t="n">
-        <f aca="false">'General Information'!B9</f>
-        <v>1234</v>
+        <v>696969</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="19"/>
@@ -1266,12 +1278,12 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C29" s="19"/>
       <c r="D29" s="19"/>
@@ -1285,12 +1297,12 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="19"/>
@@ -1304,12 +1316,12 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="18" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
@@ -1323,12 +1335,12 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C35" s="19"/>
       <c r="D35" s="19"/>
@@ -1342,12 +1354,12 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C37" s="19"/>
       <c r="D37" s="19"/>
@@ -1361,12 +1373,12 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C39" s="19"/>
       <c r="D39" s="19"/>
@@ -1380,12 +1392,12 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C41" s="19"/>
       <c r="D41" s="19"/>
@@ -1399,12 +1411,12 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C43" s="19"/>
       <c r="D43" s="19"/>
@@ -1418,12 +1430,12 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C45" s="19"/>
       <c r="D45" s="19"/>
@@ -1437,12 +1449,12 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="18" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C47" s="19"/>
       <c r="D47" s="19"/>
@@ -1456,12 +1468,12 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C49" s="19"/>
       <c r="D49" s="19"/>
@@ -1475,12 +1487,12 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C51" s="19"/>
       <c r="D51" s="19"/>
@@ -1494,12 +1506,12 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C53" s="19"/>
       <c r="D53" s="19"/>
@@ -1513,12 +1525,12 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C55" s="19"/>
       <c r="D55" s="19"/>
@@ -1532,12 +1544,12 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C57" s="19"/>
       <c r="D57" s="19"/>
@@ -1551,12 +1563,12 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="18" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C59" s="19"/>
       <c r="D59" s="19"/>
@@ -1570,12 +1582,12 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C61" s="19"/>
       <c r="D61" s="19"/>
@@ -1589,12 +1601,12 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C63" s="19"/>
       <c r="D63" s="19"/>
@@ -1608,12 +1620,12 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="18" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C65" s="19"/>
       <c r="D65" s="19"/>
@@ -1627,7 +1639,7 @@
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C66" s="21" t="n">
         <f aca="false">SUM(C2:C65)</f>

</xml_diff>

<commit_message>
Ajout de plus de détails conernant les cds
Modification du template en conséquence.
</commit_message>
<xml_diff>
--- a/files/templateEdit.xlsx
+++ b/files/templateEdit.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="110">
   <si>
     <t xml:space="preserve">Information</t>
   </si>
@@ -212,25 +212,37 @@
     <t xml:space="preserve">GAC</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of cds sequences</t>
+    <t xml:space="preserve">Nombre total de CDS</t>
   </si>
   <si>
     <t xml:space="preserve">TAC</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of invalid cds</t>
+    <t xml:space="preserve">Nombre CDS mal formé</t>
   </si>
   <si>
     <t xml:space="preserve">AAG</t>
   </si>
   <si>
+    <t xml:space="preserve">Nombre CDS identique à d’autres</t>
+  </si>
+  <si>
     <t xml:space="preserve">CAG</t>
   </si>
   <si>
+    <t xml:space="preserve">Nombre CDS restants</t>
+  </si>
+  <si>
     <t xml:space="preserve">GAG</t>
   </si>
   <si>
+    <t xml:space="preserve">Nombre CDS invalides</t>
+  </si>
+  <si>
     <t xml:space="preserve">TAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre CDS traité</t>
   </si>
   <si>
     <t xml:space="preserve">AAT</t>
@@ -349,7 +361,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY/MM/DD"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -377,6 +389,11 @@
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -500,7 +517,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -590,6 +607,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -678,12 +699,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8673469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -822,28 +843,28 @@
   </sheetPr>
   <dimension ref="A1:T66"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N26" activeCellId="0" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.780612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0561224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6377551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.1938775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.780612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="12.9132653061225"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.5"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.780612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.780612244898"/>
-    <col collapsed="false" hidden="false" max="20" min="16" style="0" width="12.9132653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="29.3112244897959"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="20" min="16" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1257,14 +1278,20 @@
         <v>696969</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="M26" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="N26" s="18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="19"/>
@@ -1275,15 +1302,27 @@
       <c r="I27" s="19"/>
       <c r="J27" s="19"/>
       <c r="K27" s="19"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M27" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="N27" s="18" t="n">
+        <v>696969</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
+      </c>
+      <c r="M28" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="N28" s="18" t="n">
+        <v>42424242</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="18" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C29" s="19"/>
       <c r="D29" s="19"/>
@@ -1294,15 +1333,21 @@
       <c r="I29" s="19"/>
       <c r="J29" s="19"/>
       <c r="K29" s="19"/>
+      <c r="M29" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="N29" s="18" t="n">
+        <v>696969</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="18" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="19"/>
@@ -1316,12 +1361,12 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="18" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
@@ -1335,12 +1380,12 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="18" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C35" s="19"/>
       <c r="D35" s="19"/>
@@ -1354,12 +1399,12 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="18" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C37" s="19"/>
       <c r="D37" s="19"/>
@@ -1373,12 +1418,12 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="18" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C39" s="19"/>
       <c r="D39" s="19"/>
@@ -1392,12 +1437,12 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="18" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C41" s="19"/>
       <c r="D41" s="19"/>
@@ -1411,12 +1456,12 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="18" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C43" s="19"/>
       <c r="D43" s="19"/>
@@ -1430,12 +1475,12 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="18" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C45" s="19"/>
       <c r="D45" s="19"/>
@@ -1449,12 +1494,12 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="18" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C47" s="19"/>
       <c r="D47" s="19"/>
@@ -1468,12 +1513,12 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="18" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C49" s="19"/>
       <c r="D49" s="19"/>
@@ -1487,12 +1532,12 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="18" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C51" s="19"/>
       <c r="D51" s="19"/>
@@ -1506,12 +1551,12 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="18" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C53" s="19"/>
       <c r="D53" s="19"/>
@@ -1525,12 +1570,12 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="18" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C55" s="19"/>
       <c r="D55" s="19"/>
@@ -1544,12 +1589,12 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="18" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C57" s="19"/>
       <c r="D57" s="19"/>
@@ -1563,12 +1608,12 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="18" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C59" s="19"/>
       <c r="D59" s="19"/>
@@ -1582,12 +1627,12 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="18" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C61" s="19"/>
       <c r="D61" s="19"/>
@@ -1601,12 +1646,12 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="18" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C63" s="19"/>
       <c r="D63" s="19"/>
@@ -1620,12 +1665,12 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="18" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C65" s="19"/>
       <c r="D65" s="19"/>

</xml_diff>

<commit_message>
Correction du template : frequence à deux décimales
Correction du nom de dossier dans Utils
</commit_message>
<xml_diff>
--- a/files/templateEdit.xlsx
+++ b/files/templateEdit.xlsx
@@ -357,11 +357,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY/MM/DD"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -389,11 +390,6 @@
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -517,7 +513,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -586,6 +582,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -598,6 +598,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -607,10 +611,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -694,17 +694,15 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.2602040816326"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.8316326530612"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -843,28 +841,26 @@
   </sheetPr>
   <dimension ref="A1:T66"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N26" activeCellId="0" sqref="N26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="29.3112244897959"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="20" min="16" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="35.1530612244898"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="20" min="16" style="0" width="12.4183673469388"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -924,325 +920,374 @@
       <c r="B2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="D2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="N2" s="18" t="s">
         <v>23</v>
       </c>
+      <c r="P2" s="17"/>
+      <c r="R2" s="17"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
       <c r="N3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="19"/>
-      <c r="T3" s="19"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="17" t="s">
+      <c r="D4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="N4" s="18" t="s">
         <v>27</v>
       </c>
+      <c r="P4" s="17"/>
+      <c r="R4" s="17"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
       <c r="N5" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="N6" s="17" t="s">
+      <c r="D6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="N6" s="18" t="s">
         <v>31</v>
       </c>
+      <c r="P6" s="17"/>
+      <c r="R6" s="17"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
       <c r="N7" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="19"/>
-      <c r="S7" s="19"/>
-      <c r="T7" s="19"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="N8" s="17" t="s">
+      <c r="D8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="N8" s="18" t="s">
         <v>35</v>
       </c>
+      <c r="P8" s="17"/>
+      <c r="R8" s="17"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
       <c r="N9" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="19"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="N10" s="17" t="s">
+      <c r="D10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="N10" s="18" t="s">
         <v>39</v>
       </c>
+      <c r="P10" s="17"/>
+      <c r="R10" s="17"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
       <c r="N11" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="19"/>
-      <c r="T11" s="19"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="20"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="N12" s="17" t="s">
+      <c r="D12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="N12" s="18" t="s">
         <v>43</v>
       </c>
+      <c r="P12" s="17"/>
+      <c r="R12" s="17"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
       <c r="N13" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="19"/>
-      <c r="S13" s="19"/>
-      <c r="T13" s="19"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="20"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N14" s="17" t="s">
+      <c r="D14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="N14" s="18" t="s">
         <v>47</v>
       </c>
+      <c r="P14" s="17"/>
+      <c r="R14" s="17"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
       <c r="N15" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="O15" s="19"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="19"/>
-      <c r="S15" s="19"/>
-      <c r="T15" s="19"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="20"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="N16" s="17" t="s">
+      <c r="D16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="N16" s="18" t="s">
         <v>51</v>
       </c>
+      <c r="P16" s="17"/>
+      <c r="R16" s="17"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
       <c r="N17" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="O17" s="19"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="19"/>
-      <c r="S17" s="19"/>
-      <c r="T17" s="19"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="20"/>
+      <c r="T17" s="20"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
         <v>54</v>
       </c>
+      <c r="D18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="H18" s="17"/>
       <c r="N18" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="O18" s="21" t="n">
+      <c r="O18" s="23" t="n">
         <f aca="false">SUM(O2:O17)</f>
         <v>0</v>
       </c>
-      <c r="P18" s="21" t="n">
+      <c r="P18" s="23" t="n">
         <f aca="false">SUM(P2:P17)</f>
         <v>0</v>
       </c>
-      <c r="Q18" s="21" t="n">
+      <c r="Q18" s="23" t="n">
         <f aca="false">SUM(Q2:Q17)</f>
         <v>0</v>
       </c>
-      <c r="R18" s="21" t="n">
+      <c r="R18" s="23" t="n">
         <f aca="false">SUM(R2:R17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
         <v>57</v>
       </c>
+      <c r="D20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="H20" s="17"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>59</v>
       </c>
+      <c r="D22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="H22" s="17"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
       <c r="M23" s="15" t="s">
         <v>61</v>
       </c>
@@ -1251,30 +1296,33 @@
       <c r="B24" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="M24" s="22" t="s">
+      <c r="D24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="M24" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="N24" s="18" t="n">
+      <c r="N24" s="19" t="n">
         <v>42424242</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="M25" s="22" t="s">
+      <c r="C25" s="20"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="M25" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="N25" s="18" t="n">
+      <c r="N25" s="19" t="n">
         <v>696969</v>
       </c>
     </row>
@@ -1282,30 +1330,33 @@
       <c r="B26" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="M26" s="23" t="s">
+      <c r="D26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="M26" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="N26" s="18" t="n">
+      <c r="N26" s="19" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="M27" s="22" t="s">
+      <c r="C27" s="20"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="M27" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="N27" s="18" t="n">
+      <c r="N27" s="19" t="n">
         <v>696969</v>
       </c>
     </row>
@@ -1313,30 +1364,33 @@
       <c r="B28" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="M28" s="22" t="s">
+      <c r="D28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="M28" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="N28" s="18" t="n">
+      <c r="N28" s="19" t="n">
         <v>42424242</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="M29" s="22" t="s">
+      <c r="C29" s="20"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="M29" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="N29" s="18" t="n">
+      <c r="N29" s="19" t="n">
         <v>696969</v>
       </c>
     </row>
@@ -1344,369 +1398,423 @@
       <c r="B30" s="0" t="s">
         <v>74</v>
       </c>
+      <c r="D30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="H30" s="17"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
         <v>76</v>
       </c>
+      <c r="D32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="H32" s="17"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
         <v>78</v>
       </c>
+      <c r="D34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="H34" s="17"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
         <v>80</v>
       </c>
+      <c r="D36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="H36" s="17"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
         <v>82</v>
       </c>
+      <c r="D38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="H38" s="17"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="D40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="H40" s="17"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
         <v>86</v>
       </c>
+      <c r="D42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="H42" s="17"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="18" t="s">
+      <c r="B43" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
         <v>88</v>
       </c>
+      <c r="D44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="H44" s="17"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="18" t="s">
+      <c r="B45" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="19"/>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
-      <c r="K45" s="19"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
         <v>90</v>
       </c>
+      <c r="D46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="H46" s="17"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="19"/>
-      <c r="H47" s="19"/>
-      <c r="I47" s="19"/>
-      <c r="J47" s="19"/>
-      <c r="K47" s="19"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="20"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
         <v>92</v>
       </c>
+      <c r="D48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="H48" s="17"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="18" t="s">
+      <c r="B49" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="19"/>
-      <c r="H49" s="19"/>
-      <c r="I49" s="19"/>
-      <c r="J49" s="19"/>
-      <c r="K49" s="19"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="20"/>
+      <c r="J49" s="20"/>
+      <c r="K49" s="20"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
         <v>94</v>
       </c>
+      <c r="D50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="H50" s="17"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="18" t="s">
+      <c r="B51" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="19"/>
-      <c r="H51" s="19"/>
-      <c r="I51" s="19"/>
-      <c r="J51" s="19"/>
-      <c r="K51" s="19"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="20"/>
+      <c r="J51" s="20"/>
+      <c r="K51" s="20"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
         <v>96</v>
       </c>
+      <c r="D52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="H52" s="17"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="18" t="s">
+      <c r="B53" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="19"/>
-      <c r="I53" s="19"/>
-      <c r="J53" s="19"/>
-      <c r="K53" s="19"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="20"/>
+      <c r="J53" s="20"/>
+      <c r="K53" s="20"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
         <v>98</v>
       </c>
+      <c r="D54" s="17"/>
+      <c r="F54" s="17"/>
+      <c r="H54" s="17"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="18" t="s">
+      <c r="B55" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="19"/>
-      <c r="H55" s="19"/>
-      <c r="I55" s="19"/>
-      <c r="J55" s="19"/>
-      <c r="K55" s="19"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="21"/>
+      <c r="I55" s="20"/>
+      <c r="J55" s="20"/>
+      <c r="K55" s="20"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
         <v>100</v>
       </c>
+      <c r="D56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="H56" s="17"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="18" t="s">
+      <c r="B57" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="C57" s="19"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="19"/>
-      <c r="H57" s="19"/>
-      <c r="I57" s="19"/>
-      <c r="J57" s="19"/>
-      <c r="K57" s="19"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="21"/>
+      <c r="I57" s="20"/>
+      <c r="J57" s="20"/>
+      <c r="K57" s="20"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
         <v>102</v>
       </c>
+      <c r="D58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="H58" s="17"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="18" t="s">
+      <c r="B59" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="C59" s="19"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="19"/>
-      <c r="F59" s="19"/>
-      <c r="G59" s="19"/>
-      <c r="H59" s="19"/>
-      <c r="I59" s="19"/>
-      <c r="J59" s="19"/>
-      <c r="K59" s="19"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="20"/>
+      <c r="J59" s="20"/>
+      <c r="K59" s="20"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
         <v>104</v>
       </c>
+      <c r="D60" s="17"/>
+      <c r="F60" s="17"/>
+      <c r="H60" s="17"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="18" t="s">
+      <c r="B61" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="C61" s="19"/>
-      <c r="D61" s="19"/>
-      <c r="E61" s="19"/>
-      <c r="F61" s="19"/>
-      <c r="G61" s="19"/>
-      <c r="H61" s="19"/>
-      <c r="I61" s="19"/>
-      <c r="J61" s="19"/>
-      <c r="K61" s="19"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="21"/>
+      <c r="G61" s="20"/>
+      <c r="H61" s="21"/>
+      <c r="I61" s="20"/>
+      <c r="J61" s="20"/>
+      <c r="K61" s="20"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
         <v>106</v>
       </c>
+      <c r="D62" s="17"/>
+      <c r="F62" s="17"/>
+      <c r="H62" s="17"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="18" t="s">
+      <c r="B63" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="C63" s="19"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="19"/>
-      <c r="F63" s="19"/>
-      <c r="G63" s="19"/>
-      <c r="H63" s="19"/>
-      <c r="I63" s="19"/>
-      <c r="J63" s="19"/>
-      <c r="K63" s="19"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="20"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="20"/>
+      <c r="H63" s="21"/>
+      <c r="I63" s="20"/>
+      <c r="J63" s="20"/>
+      <c r="K63" s="20"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="s">
         <v>108</v>
       </c>
+      <c r="D64" s="17"/>
+      <c r="F64" s="17"/>
+      <c r="H64" s="17"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="18" t="s">
+      <c r="B65" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C65" s="19"/>
-      <c r="D65" s="19"/>
-      <c r="E65" s="19"/>
-      <c r="F65" s="19"/>
-      <c r="G65" s="19"/>
-      <c r="H65" s="19"/>
-      <c r="I65" s="19"/>
-      <c r="J65" s="19"/>
-      <c r="K65" s="19"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="21"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="21"/>
+      <c r="I65" s="20"/>
+      <c r="J65" s="20"/>
+      <c r="K65" s="20"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C66" s="21" t="n">
+      <c r="C66" s="23" t="n">
         <f aca="false">SUM(C2:C65)</f>
         <v>0</v>
       </c>
-      <c r="D66" s="21" t="n">
+      <c r="D66" s="23" t="n">
         <f aca="false">SUM(D2:D65)</f>
         <v>0</v>
       </c>
-      <c r="E66" s="21" t="n">
+      <c r="E66" s="23" t="n">
         <f aca="false">SUM(E2:E65)</f>
         <v>0</v>
       </c>
-      <c r="F66" s="21" t="n">
+      <c r="F66" s="23" t="n">
         <f aca="false">SUM(F2:F65)</f>
         <v>0</v>
       </c>
-      <c r="G66" s="21" t="n">
+      <c r="G66" s="23" t="n">
         <f aca="false">SUM(G2:G65)</f>
         <v>0</v>
       </c>
-      <c r="H66" s="21" t="n">
+      <c r="H66" s="23" t="n">
         <f aca="false">SUM(H2:H65)</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Fix + MAJ gérée
</commit_message>
<xml_diff>
--- a/files/templateEdit.xlsx
+++ b/files/templateEdit.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="1" state="visible" r:id="rId2"/>
@@ -357,7 +357,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY/MM/DD"/>
-    <numFmt numFmtId="166" formatCode="0.00"/>
+    <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -510,7 +510,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -604,6 +604,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -690,18 +694,18 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.9540816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.4591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -840,28 +844,32 @@
   </sheetPr>
   <dimension ref="A1:T66"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="20" min="16" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.234693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="20" min="19" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1219,7 +1227,7 @@
         <f aca="false">SUM(O2:O17)</f>
         <v>0</v>
       </c>
-      <c r="P18" s="23" t="n">
+      <c r="P18" s="24" t="n">
         <f aca="false">SUM(P2:P17)</f>
         <v>0</v>
       </c>
@@ -1227,7 +1235,7 @@
         <f aca="false">SUM(Q2:Q17)</f>
         <v>0</v>
       </c>
-      <c r="R18" s="23" t="n">
+      <c r="R18" s="24" t="n">
         <f aca="false">SUM(R2:R17)</f>
         <v>0</v>
       </c>
@@ -1300,7 +1308,7 @@
       <c r="D24" s="17"/>
       <c r="F24" s="17"/>
       <c r="H24" s="17"/>
-      <c r="M24" s="24" t="s">
+      <c r="M24" s="25" t="s">
         <v>63</v>
       </c>
       <c r="N24" s="19" t="n">
@@ -1320,7 +1328,7 @@
       <c r="I25" s="20"/>
       <c r="J25" s="20"/>
       <c r="K25" s="20"/>
-      <c r="M25" s="24" t="s">
+      <c r="M25" s="25" t="s">
         <v>65</v>
       </c>
       <c r="N25" s="19" t="n">
@@ -1334,7 +1342,7 @@
       <c r="D26" s="17"/>
       <c r="F26" s="17"/>
       <c r="H26" s="17"/>
-      <c r="M26" s="24" t="s">
+      <c r="M26" s="25" t="s">
         <v>67</v>
       </c>
       <c r="N26" s="19" t="n">
@@ -1354,7 +1362,7 @@
       <c r="I27" s="20"/>
       <c r="J27" s="20"/>
       <c r="K27" s="20"/>
-      <c r="M27" s="24" t="s">
+      <c r="M27" s="25" t="s">
         <v>69</v>
       </c>
       <c r="N27" s="19" t="n">
@@ -1368,7 +1376,7 @@
       <c r="D28" s="17"/>
       <c r="F28" s="17"/>
       <c r="H28" s="17"/>
-      <c r="M28" s="24" t="s">
+      <c r="M28" s="25" t="s">
         <v>71</v>
       </c>
       <c r="N28" s="19" t="n">
@@ -1785,7 +1793,7 @@
       <c r="J65" s="20"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="15" t="s">
         <v>55</v>
       </c>
@@ -1793,7 +1801,7 @@
         <f aca="false">SUM(C2:C65)</f>
         <v>0</v>
       </c>
-      <c r="D66" s="23" t="n">
+      <c r="D66" s="24" t="n">
         <f aca="false">SUM(D2:D65)</f>
         <v>0</v>
       </c>
@@ -1801,7 +1809,7 @@
         <f aca="false">SUM(E2:E65)</f>
         <v>0</v>
       </c>
-      <c r="F66" s="23" t="n">
+      <c r="F66" s="24" t="n">
         <f aca="false">SUM(F2:F65)</f>
         <v>0</v>
       </c>
@@ -1809,7 +1817,7 @@
         <f aca="false">SUM(G2:G65)</f>
         <v>0</v>
       </c>
-      <c r="H66" s="23" t="n">
+      <c r="H66" s="24" t="n">
         <f aca="false">SUM(H2:H65)</f>
         <v>0</v>
       </c>

</xml_diff>